<commit_message>
Added burndown chart and sprint backlog for second sprint
</commit_message>
<xml_diff>
--- a/sprints/sprint 2/Burndown Chart Sprint 1.xlsx
+++ b/sprints/sprint 2/Burndown Chart Sprint 1.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\Uni Stuff\UWI\Semester 4\COMP 3613\Group Project\swe2-project\sprints\sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azeldaniel/Documents/UWI/Year 3/Semester 1/COMP 3613/project/swe2-project/sprints/sprint 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43C2D89-63BD-3C4E-9C4E-AD6FC2E7EC4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8415" xr2:uid="{583FEC89-0C8D-4923-A5A2-4ADAB6A20CAF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{583FEC89-0C8D-4923-A5A2-4ADAB6A20CAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -219,67 +225,31 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>43384</c:v>
+                  <c:v>43416</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43385</c:v>
+                  <c:v>43417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43386</c:v>
+                  <c:v>43418</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43387</c:v>
+                  <c:v>43419</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43388</c:v>
+                  <c:v>43420</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43389</c:v>
+                  <c:v>43421</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43390</c:v>
+                  <c:v>43422</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43391</c:v>
+                  <c:v>43423</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43392</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43393</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43394</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43395</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43396</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43397</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43398</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43399</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43400</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43401</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43402</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43403</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43404</c:v>
+                  <c:v>43424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -291,67 +261,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,67 +306,31 @@
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>43384</c:v>
+                  <c:v>43416</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43385</c:v>
+                  <c:v>43417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43386</c:v>
+                  <c:v>43418</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43387</c:v>
+                  <c:v>43419</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43388</c:v>
+                  <c:v>43420</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43389</c:v>
+                  <c:v>43421</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43390</c:v>
+                  <c:v>43422</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43391</c:v>
+                  <c:v>43423</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43392</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43393</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43394</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43395</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43396</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43397</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43398</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43399</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43400</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43401</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43402</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43403</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43404</c:v>
+                  <c:v>43424</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -468,67 +342,31 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>66</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.7</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.400000000000006</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.100000000000009</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.800000000000011</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.500000000000014</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46.200000000000017</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.90000000000002</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39.600000000000023</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>36.300000000000026</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>33.000000000000028</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29.700000000000028</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26.400000000000027</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>23.100000000000026</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>19.800000000000026</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.500000000000025</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13.200000000000024</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9.9000000000000234</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.6000000000000236</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.3000000000000238</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.3980817331903381E-14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1638,17 +1476,17 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1662,59 +1500,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43384</v>
+        <v>43416</v>
       </c>
       <c r="B2">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="U2" t="s">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W2" s="2">
         <f>(V2/7)</f>
-        <v>1.8571428571428572</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43385</v>
-      </c>
-      <c r="B3">
-        <v>65</v>
+        <v>43417</v>
       </c>
       <c r="C3" s="3">
-        <f>(C2-3.3)</f>
-        <v>62.7</v>
+        <f>C2-9</f>
+        <v>63</v>
       </c>
       <c r="U3" t="s">
         <v>1</v>
       </c>
       <c r="V3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="W3" s="2">
         <f t="shared" ref="W3:W6" si="0">(V3/7)</f>
-        <v>2.2857142857142856</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+        <v>2.4285714285714284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43386</v>
-      </c>
-      <c r="B4">
-        <v>65</v>
+        <v>43418</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ref="C4:C22" si="1">(C3-3.3)</f>
-        <v>59.400000000000006</v>
+        <f t="shared" ref="C4:C10" si="1">C3-9</f>
+        <v>54</v>
       </c>
       <c r="U4" t="s">
         <v>2</v>
@@ -1727,284 +1559,170 @@
         <v>1.5714285714285714</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43387</v>
-      </c>
-      <c r="B5">
-        <v>65</v>
+        <v>43419</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="1"/>
-        <v>56.100000000000009</v>
+        <v>45</v>
       </c>
       <c r="U5" t="s">
         <v>3</v>
       </c>
       <c r="V5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="W5" s="2">
         <f t="shared" si="0"/>
-        <v>1.4285714285714286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+        <v>2.1428571428571428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43388</v>
-      </c>
-      <c r="B6">
-        <v>61</v>
+        <v>43420</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="1"/>
-        <v>52.800000000000011</v>
+        <v>36</v>
       </c>
       <c r="U6" t="s">
         <v>4</v>
       </c>
       <c r="V6">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="W6" s="2">
         <f t="shared" si="0"/>
-        <v>2.2857142857142856</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+        <v>1.5714285714285714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43389</v>
-      </c>
-      <c r="B7">
-        <v>61</v>
+        <v>43421</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="1"/>
-        <v>49.500000000000014</v>
+        <v>27</v>
       </c>
       <c r="V7">
         <f>SUM(V2:V6)</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="W7" s="2">
         <f>(SUM(W2:W6)/5)</f>
-        <v>1.8857142857142855</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+        <v>1.9428571428571426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43390</v>
-      </c>
-      <c r="B8">
-        <v>59</v>
+        <v>43422</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="1"/>
-        <v>46.200000000000017</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43391</v>
-      </c>
-      <c r="B9">
-        <v>59</v>
+        <v>43423</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="1"/>
-        <v>42.90000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43392</v>
-      </c>
-      <c r="B10">
-        <v>59</v>
+        <v>43424</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="1"/>
-        <v>39.600000000000023</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>43393</v>
-      </c>
-      <c r="B11">
-        <v>59</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" si="1"/>
-        <v>36.300000000000026</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>43394</v>
-      </c>
-      <c r="B12">
-        <v>59</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" si="1"/>
-        <v>33.000000000000028</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>43395</v>
-      </c>
-      <c r="B13">
-        <v>59</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="1"/>
-        <v>29.700000000000028</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>43396</v>
-      </c>
-      <c r="B14">
-        <v>59</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" si="1"/>
-        <v>26.400000000000027</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>43397</v>
-      </c>
-      <c r="B15">
-        <v>59</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="1"/>
-        <v>23.100000000000026</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>43398</v>
-      </c>
-      <c r="B16">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3">
-        <f t="shared" si="1"/>
-        <v>19.800000000000026</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>43399</v>
-      </c>
-      <c r="B17">
-        <v>25</v>
-      </c>
-      <c r="C17" s="3">
-        <f t="shared" si="1"/>
-        <v>16.500000000000025</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>43400</v>
-      </c>
-      <c r="B18">
-        <v>11</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="1"/>
-        <v>13.200000000000024</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>43401</v>
-      </c>
-      <c r="B19">
-        <v>11</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="1"/>
-        <v>9.9000000000000234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>43402</v>
-      </c>
-      <c r="B20">
         <v>0</v>
       </c>
-      <c r="C20" s="3">
-        <f t="shared" si="1"/>
-        <v>6.6000000000000236</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>43403</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" si="1"/>
-        <v>3.3000000000000238</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>43404</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" s="3">
-        <f t="shared" si="1"/>
-        <v>2.3980817331903381E-14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
     </row>
   </sheetData>

</xml_diff>